<commit_message>
Resize deck builder cards on PC and update version to 3.3.1
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ss\ss\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E466B4F-F651-493E-8A2E-A6DD09E9A465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1334F12D-69F6-47DD-A391-4E6DD4A6FEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -1747,7 +1747,7 @@
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="18">
     <dxf>
       <border>
         <bottom style="dashed">
@@ -1756,6 +1756,34 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -1873,61 +1901,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="dashed">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="dashed">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="dashed">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -8938,8 +8911,8 @@
   <dimension ref="A1:H841"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A568" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G824" sqref="G824"/>
+      <pane ySplit="1" topLeftCell="A805" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K825" sqref="K825"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -25394,237 +25367,237 @@
         <v>54</v>
       </c>
     </row>
-    <row r="634" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A634">
+    <row r="634" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A634" s="4">
         <v>29</v>
       </c>
-      <c r="B634" t="s">
+      <c r="B634" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C634" t="s">
+      <c r="C634" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D634" t="s">
-        <v>435</v>
-      </c>
-      <c r="E634" t="s">
-        <v>54</v>
-      </c>
-      <c r="F634" t="s">
-        <v>436</v>
-      </c>
-      <c r="G634" s="1" t="s">
+      <c r="D634" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E634" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F634" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G634" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H634" s="1" t="s">
+      <c r="H634" s="5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="635" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A635">
+    <row r="635" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A635" s="4">
         <v>29</v>
       </c>
-      <c r="B635" t="s">
+      <c r="B635" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C635" t="s">
+      <c r="C635" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D635" t="s">
-        <v>435</v>
-      </c>
-      <c r="E635" t="s">
-        <v>54</v>
-      </c>
-      <c r="F635" t="s">
-        <v>436</v>
-      </c>
-      <c r="G635" s="1" t="s">
+      <c r="D635" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E635" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F635" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G635" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="H635" s="1" t="s">
+      <c r="H635" s="5" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="636" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A636">
+    <row r="636" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A636" s="4">
         <v>29</v>
       </c>
-      <c r="B636" t="s">
+      <c r="B636" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C636" t="s">
+      <c r="C636" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D636" t="s">
-        <v>435</v>
-      </c>
-      <c r="E636" t="s">
-        <v>54</v>
-      </c>
-      <c r="F636" t="s">
-        <v>436</v>
-      </c>
-      <c r="G636" s="1" t="s">
+      <c r="D636" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E636" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F636" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G636" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="H636" s="1" t="s">
+      <c r="H636" s="5" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="637" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A637">
+    <row r="637" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A637" s="4">
         <v>29</v>
       </c>
-      <c r="B637" t="s">
+      <c r="B637" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C637" t="s">
+      <c r="C637" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D637" t="s">
-        <v>435</v>
-      </c>
-      <c r="E637" t="s">
-        <v>54</v>
-      </c>
-      <c r="F637" t="s">
-        <v>436</v>
-      </c>
-      <c r="G637" s="1" t="s">
+      <c r="D637" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E637" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F637" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G637" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="H637" s="1" t="s">
+      <c r="H637" s="5" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="638" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A638">
+    <row r="638" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A638" s="4">
         <v>29</v>
       </c>
-      <c r="B638" t="s">
+      <c r="B638" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C638" t="s">
+      <c r="C638" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D638" t="s">
-        <v>435</v>
-      </c>
-      <c r="E638" t="s">
-        <v>54</v>
-      </c>
-      <c r="F638" t="s">
+      <c r="D638" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E638" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F638" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="G638" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H638" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="639" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A639">
+      <c r="G638" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H638" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="639" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A639" s="4">
         <v>29</v>
       </c>
-      <c r="B639" t="s">
+      <c r="B639" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C639" t="s">
+      <c r="C639" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D639" t="s">
-        <v>435</v>
-      </c>
-      <c r="E639" t="s">
-        <v>54</v>
-      </c>
-      <c r="F639" t="s">
+      <c r="D639" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E639" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F639" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="G639" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H639" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="640" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A640">
+      <c r="G639" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H639" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="640" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A640" s="4">
         <v>29</v>
       </c>
-      <c r="B640" t="s">
+      <c r="B640" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C640" t="s">
+      <c r="C640" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D640" t="s">
-        <v>440</v>
-      </c>
-      <c r="E640" t="s">
-        <v>54</v>
-      </c>
-      <c r="F640" t="s">
-        <v>436</v>
-      </c>
-      <c r="G640" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H640" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="641" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A641">
+      <c r="D640" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="E640" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F640" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="G640" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H640" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="641" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A641" s="4">
         <v>29</v>
       </c>
-      <c r="B641" t="s">
+      <c r="B641" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C641" t="s">
+      <c r="C641" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D641" t="s">
-        <v>440</v>
-      </c>
-      <c r="E641" t="s">
-        <v>54</v>
-      </c>
-      <c r="F641" t="s">
+      <c r="D641" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="E641" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F641" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="G641" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H641" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="642" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A642">
+      <c r="G641" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H641" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="642" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A642" s="4">
         <v>29</v>
       </c>
-      <c r="B642" t="s">
+      <c r="B642" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C642" t="s">
+      <c r="C642" s="4" t="s">
         <v>434</v>
       </c>
-      <c r="D642" t="s">
-        <v>440</v>
-      </c>
-      <c r="E642" t="s">
-        <v>54</v>
-      </c>
-      <c r="F642" t="s">
+      <c r="D642" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="E642" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F642" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="G642" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H642" s="1" t="s">
+      <c r="G642" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H642" s="5" t="s">
         <v>54</v>
       </c>
     </row>
@@ -30746,105 +30719,90 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
-      <formula>"선택지B"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
-      <formula>"선택지A"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H88 A92:H92 A656:H656 A659:H682 A94:H393 A395:H644 A793:H1048569 A685:H789">
-    <cfRule type="expression" dxfId="18" priority="18">
+  <conditionalFormatting sqref="A2:H88 A94:H393 A395:H644 A656:H656 A659:H682">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$C3&lt;&gt;$C2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
-      <formula>"실패"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
-      <formula>"성공"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A683:H683 D684 A657:H657 A658:F658 A649:H649">
-    <cfRule type="expression" dxfId="15" priority="23">
-      <formula>$C651&lt;&gt;$C649</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A684:H684">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>$C685&lt;&gt;$C684</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A89:H89 A646:H646">
-    <cfRule type="expression" dxfId="13" priority="26">
+    <cfRule type="expression" dxfId="16" priority="26">
       <formula>$C92&lt;&gt;$C89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A90:H90">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="15" priority="14">
       <formula>$C92&lt;&gt;$C90</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A91:H91">
-    <cfRule type="expression" dxfId="11" priority="13">
+  <conditionalFormatting sqref="A91:H92">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>$C92&lt;&gt;$C91</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A93:H93 A655:H655 A651:H652 A645:H645 A394:H394 A791:H791">
-    <cfRule type="expression" dxfId="10" priority="35">
+  <conditionalFormatting sqref="A93:H93 A394:H394 A645:H645 A655:H655">
+    <cfRule type="expression" dxfId="13" priority="35">
       <formula>#REF!&lt;&gt;$C93</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A654:H654">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>$C655&lt;&gt;$C654</formula>
+  <conditionalFormatting sqref="A647:H648">
+    <cfRule type="expression" dxfId="12" priority="7">
+      <formula>$C648&lt;&gt;$C647</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A653:H653">
-    <cfRule type="expression" dxfId="8" priority="10">
+  <conditionalFormatting sqref="A649:H649 A657:H657 A658:F658 A683:H683 D684">
+    <cfRule type="expression" dxfId="11" priority="23">
+      <formula>$C651&lt;&gt;$C649</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A650:H652">
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>#REF!&lt;&gt;$C650</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A653:H654">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$C654&lt;&gt;$C653</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G658:H658">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>#REF!&lt;&gt;$C658</formula>
+  <conditionalFormatting sqref="A684:H789">
+    <cfRule type="expression" dxfId="8" priority="15">
+      <formula>$C685&lt;&gt;$C684</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A648:H648">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>$C649&lt;&gt;$C648</formula>
+  <conditionalFormatting sqref="A790:H791">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>#REF!&lt;&gt;$C790</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A647:H647">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>$C648&lt;&gt;$C647</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A650:H650">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>#REF!&lt;&gt;$C650</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A792:F792">
-    <cfRule type="expression" dxfId="3" priority="4">
+  <conditionalFormatting sqref="A792:H1048569">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$C793&lt;&gt;$C792</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G792:H792">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$C793&lt;&gt;$C792</formula>
+  <conditionalFormatting sqref="A1048570:H1048576">
+    <cfRule type="expression" dxfId="5" priority="114">
+      <formula>$C1&lt;&gt;$C1048570</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A790:H790">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>#REF!&lt;&gt;$C790</formula>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
+      <formula>"선택지B"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"선택지A"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1048570:H1048576">
-    <cfRule type="expression" dxfId="0" priority="114">
-      <formula>$C1&lt;&gt;$C1048570</formula>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
+      <formula>"실패"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
+      <formula>"성공"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G658:H658">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>#REF!&lt;&gt;$C658</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>